<commit_message>
test cases of epoch validator
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anand\gitControl\JenkinsIntegrationWithGit\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anand\gitControl\EpochValidatorSuite\EpochValidatorSuite\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2EE607-D4B2-4298-ACA9-0A3128356B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C699DCB-8B29-457C-BEBA-3BBA345179C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BA62212C-8BEA-4AB6-98A5-F0DE0C70441F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="epochValidator" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,33 +33,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>testcase</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>loginSuccess</t>
-  </si>
-  <si>
-    <t>loginFailed</t>
-  </si>
-  <si>
-    <t>resetPassword</t>
-  </si>
-  <si>
-    <t>anand</t>
-  </si>
-  <si>
-    <t>Automation@123</t>
-  </si>
-  <si>
-    <t>emptyusername</t>
+    <t>verifyEpochConversionWithValidInput</t>
+  </si>
+  <si>
+    <t>verifyEpochConversionWithInvalidInputExceedingInt32Range</t>
+  </si>
+  <si>
+    <t>verifyEpochConversionWithInvalidInput</t>
+  </si>
+  <si>
+    <t>ExpectedMessage</t>
+  </si>
+  <si>
+    <t>UnixTimeService.RESTHost.fromunixtimestamp.TryCatch.Try.UnixTimeStamp: Input string was not in a correct format.</t>
+  </si>
+  <si>
+    <t>UnixTimeService.RESTHost.fromunixtimestamp.TryCatch.Try.UnixTimeStamp: Value was either too large or too small for an Int32.</t>
   </si>
 </sst>
 </file>
@@ -425,13 +419,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="56.21875" customWidth="1"/>
+    <col min="2" max="2" width="49.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -440,46 +434,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3">
-        <v>123456</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{DA4343D1-FD6E-4D1D-AE9F-22842BA0B4C2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>